<commit_message>
Part 0 completed, updated Timetable
</commit_message>
<xml_diff>
--- a/Timetable and status.xlsx
+++ b/Timetable and status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joona\Desktop\FullStackOpen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB2454E-C470-4FC2-9B8B-BCAEADB4E75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35795AD8-4883-4654-A70D-F5EE6077E876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="345" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,27 +35,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Osa</t>
-  </si>
-  <si>
-    <t>Tehtäviä tehty</t>
-  </si>
-  <si>
-    <t>Ajoitus (viikko)</t>
-  </si>
-  <si>
-    <t>25-26</t>
-  </si>
-  <si>
-    <t>27-28</t>
-  </si>
-  <si>
-    <t>Valmistunut viikolla</t>
-  </si>
-  <si>
-    <t>Jatketaan osan 0 tehtävistä</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>13.06.2022</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>12.06.2022</t>
+  </si>
+  <si>
+    <t>19.06.2022</t>
+  </si>
+  <si>
+    <t>3.7.2022</t>
+  </si>
+  <si>
+    <t>10.7.2022</t>
+  </si>
+  <si>
+    <t>17.7.2022</t>
+  </si>
+  <si>
+    <t>24.7.2022</t>
+  </si>
+  <si>
+    <t>31.7.2022</t>
+  </si>
+  <si>
+    <t>7.8.2022</t>
+  </si>
+  <si>
+    <t>14.8.2022</t>
+  </si>
+  <si>
+    <t>21.8.2022</t>
+  </si>
+  <si>
+    <t>28.8.2022</t>
+  </si>
+  <si>
+    <t>4.9.2022</t>
+  </si>
+  <si>
+    <t>11.9.2022</t>
+  </si>
+  <si>
+    <t>18.9.2022</t>
+  </si>
+  <si>
+    <t>Completed tasks</t>
   </si>
 </sst>
 </file>
@@ -111,13 +147,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -139,11 +175,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3BE6235-366F-47A6-A75B-9F691CBE24E6}" name="Table1" displayName="Table1" ref="B2:E17" totalsRowCount="1">
   <autoFilter ref="B2:E16" xr:uid="{F3BE6235-366F-47A6-A75B-9F691CBE24E6}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E4B41EE2-3D7D-49F5-A337-D679EF514D86}" name="Osa" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{48D8E5DE-5430-4386-A639-240D7B4A91AA}" name="Ajoitus (viikko)" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{AEDF529B-D3EC-45E4-A466-E4DEC49DC96F}" name="Valmistunut viikolla"/>
-    <tableColumn id="4" xr3:uid="{0EC6EC50-0860-475E-9316-80833B376DB9}" name="Tehtäviä tehty" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(Table1[Tehtäviä tehty])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{E4B41EE2-3D7D-49F5-A337-D679EF514D86}" name="Part" dataDxfId="5" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{48D8E5DE-5430-4386-A639-240D7B4A91AA}" name="Deadline" dataDxfId="4" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{AEDF529B-D3EC-45E4-A466-E4DEC49DC96F}" name="Finished"/>
+    <tableColumn id="4" xr3:uid="{0EC6EC50-0860-475E-9316-80833B376DB9}" name="Completed tasks" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(Table1[Completed tasks])</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -413,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G17"/>
+  <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,176 +460,176 @@
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="2">
-        <v>23</v>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
-        <v>24</v>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
-        <v>29</v>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
-        <v>30</v>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
-        <v>31</v>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
-        <v>32</v>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="E10" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>33</v>
+      <c r="C11" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
-        <v>34</v>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="E12" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
-        <v>35</v>
+      <c r="C13" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>11</v>
       </c>
-      <c r="C14" s="2">
-        <v>36</v>
+      <c r="C14" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
-        <v>37</v>
+      <c r="C15" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
-        <v>38</v>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -603,8 +639,8 @@
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="E17" s="2">
-        <f>SUM(Table1[Tehtäviä tehty])</f>
-        <v>0</v>
+        <f>SUM(Table1[Completed tasks])</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished unicafe tasks, started anecdotes
</commit_message>
<xml_diff>
--- a/Timetable and status.xlsx
+++ b/Timetable and status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joona\Desktop\FullStackOpen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35795AD8-4883-4654-A70D-F5EE6077E876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC549828-6D3C-42B6-A8E7-2105F53A3DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="345" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>13.06.2022</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>18.9.2022</t>
-  </si>
-  <si>
-    <t>Completed tasks</t>
   </si>
 </sst>
 </file>
@@ -139,7 +136,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="4">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -148,12 +145,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -172,15 +163,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3BE6235-366F-47A6-A75B-9F691CBE24E6}" name="Table1" displayName="Table1" ref="B2:E17" totalsRowCount="1">
-  <autoFilter ref="B2:E16" xr:uid="{F3BE6235-366F-47A6-A75B-9F691CBE24E6}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E4B41EE2-3D7D-49F5-A337-D679EF514D86}" name="Part" dataDxfId="5" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{48D8E5DE-5430-4386-A639-240D7B4A91AA}" name="Deadline" dataDxfId="4" totalsRowDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3BE6235-366F-47A6-A75B-9F691CBE24E6}" name="Table1" displayName="Table1" ref="B2:D17" totalsRowCount="1">
+  <autoFilter ref="B2:D16" xr:uid="{F3BE6235-366F-47A6-A75B-9F691CBE24E6}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E4B41EE2-3D7D-49F5-A337-D679EF514D86}" name="Part" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{48D8E5DE-5430-4386-A639-240D7B4A91AA}" name="Deadline" dataDxfId="1" totalsRowDxfId="0"/>
     <tableColumn id="3" xr3:uid="{AEDF529B-D3EC-45E4-A466-E4DEC49DC96F}" name="Finished"/>
-    <tableColumn id="4" xr3:uid="{0EC6EC50-0860-475E-9316-80833B376DB9}" name="Completed tasks" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="0">
-      <totalsRowFormula>SUM(Table1[Completed tasks])</totalsRowFormula>
-    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -449,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E17"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,11 +448,10 @@
     <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -474,11 +461,8 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>0</v>
       </c>
@@ -488,160 +472,114 @@
       <c r="D3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
-      <c r="E17" s="2">
-        <f>SUM(Table1[Completed tasks])</f>
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continued work on part 2
</commit_message>
<xml_diff>
--- a/Timetable and status.xlsx
+++ b/Timetable and status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joona\Desktop\FullStackOpen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC549828-6D3C-42B6-A8E7-2105F53A3DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537F42DC-C692-4162-8F1D-D399E4CDC440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>13.06.2022</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>18.9.2022</t>
+  </si>
+  <si>
+    <t>21.06.2022</t>
   </si>
 </sst>
 </file>
@@ -141,10 +144,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -166,8 +169,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3BE6235-366F-47A6-A75B-9F691CBE24E6}" name="Table1" displayName="Table1" ref="B2:D17" totalsRowCount="1">
   <autoFilter ref="B2:D16" xr:uid="{F3BE6235-366F-47A6-A75B-9F691CBE24E6}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E4B41EE2-3D7D-49F5-A337-D679EF514D86}" name="Part" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{48D8E5DE-5430-4386-A639-240D7B4A91AA}" name="Deadline" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E4B41EE2-3D7D-49F5-A337-D679EF514D86}" name="Part" dataDxfId="3" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{48D8E5DE-5430-4386-A639-240D7B4A91AA}" name="Deadline" dataDxfId="2" totalsRowDxfId="0"/>
     <tableColumn id="3" xr3:uid="{AEDF529B-D3EC-45E4-A466-E4DEC49DC96F}" name="Finished"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -440,7 +443,7 @@
   <dimension ref="B2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +483,9 @@
       <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1">

</xml_diff>